<commit_message>
New Sanity updates in Prod
</commit_message>
<xml_diff>
--- a/Input_files/Actual_testcases/Kaman/Prod/ALL_PAGES/END_TO_END/TC01_Verify_HomePage.xlsx
+++ b/Input_files/Actual_testcases/Kaman/Prod/ALL_PAGES/END_TO_END/TC01_Verify_HomePage.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KAMANLiveBranch\Input_files\Actual_testcases\Kaman\Prod\ALL_PAGES\END_TO_END\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7763A3B3-2D44-49C7-B6E4-FCFF26F19F06}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="TC01_Verify_HomePage" sheetId="1" r:id="rId1"/>
@@ -21,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="16">
   <si>
     <t>TestCase</t>
   </si>
@@ -56,9 +50,6 @@
     <t>KamanLogo</t>
   </si>
   <si>
-    <t>HomeCarousel</t>
-  </si>
-  <si>
     <t>SearchBoxHomePage</t>
   </si>
   <si>
@@ -71,34 +62,19 @@
     <t>CSS</t>
   </si>
   <si>
-    <t>EleType1</t>
-  </si>
-  <si>
-    <t>EleType2</t>
-  </si>
-  <si>
-    <t>JSElement</t>
-  </si>
-  <si>
     <t>HeroBanner</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -144,12 +120,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -495,18 +470,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.7109375" customWidth="1"/>
+    <col min="2" max="2" width="38" customWidth="1"/>
+    <col min="3" max="3" width="25" customWidth="1"/>
     <col min="4" max="4" width="15.42578125" customWidth="1"/>
     <col min="5" max="5" width="21.28515625" customWidth="1"/>
   </cols>
@@ -544,13 +519,13 @@
     <row r="3" spans="1:5">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>15</v>
+      <c r="D3" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>10</v>
@@ -559,31 +534,31 @@
     <row r="4" spans="1:5">
       <c r="A4" s="3"/>
       <c r="B4" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="4" t="s">
         <v>15</v>
       </c>
+      <c r="D4" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="E4" s="3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="3"/>
       <c r="B5" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>15</v>
+        <v>11</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -594,16 +569,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B7"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" customWidth="1"/>
+    <col min="1" max="1" width="23.42578125" customWidth="1"/>
     <col min="2" max="2" width="35.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -620,7 +595,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -633,7 +608,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B4" s="3" t="b">
         <v>1</v>
@@ -641,40 +616,27 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="3" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="https://192.168.15.18/storeus" xr:uid="{C28EA635-1DD4-4B93-B594-513E4D966091}"/>
+    <hyperlink ref="B2" r:id="rId1" display="https://192.168.15.18/storeus"/>
   </hyperlinks>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -875,19 +837,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{201F13FF-ABE4-451A-88FD-FA1FE3D91855}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75986BA1-ED37-4C63-93A8-4C325EA50F3E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -912,9 +870,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75986BA1-ED37-4C63-93A8-4C325EA50F3E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{201F13FF-ABE4-451A-88FD-FA1FE3D91855}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>